<commit_message>
added LAF test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2200106\Downloads\LAF_SMT-master (1)\LAF_SMT-master\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73123BA3-3D26-48D1-BCEA-7CF047B5C99B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D0DF901-73C3-40D4-81B6-DBB656C40A8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" tabRatio="835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="10545" windowHeight="10035" tabRatio="835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LAF" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="124">
   <si>
     <t>TestScenario</t>
   </si>
@@ -390,6 +390,27 @@
   </si>
   <si>
     <t>Check_search_textbox</t>
+  </si>
+  <si>
+    <t>TC_07_Validate_LAF_Title</t>
+  </si>
+  <si>
+    <t>TC_08_Validate_JoinNow_Button</t>
+  </si>
+  <si>
+    <t>TC_09_Validate_JoinNow_ClickButton</t>
+  </si>
+  <si>
+    <t>CheckLAF_Title</t>
+  </si>
+  <si>
+    <t>Check_LAF_JoinNowHeaderButton</t>
+  </si>
+  <si>
+    <t>Click_JoinNowHeaderButton</t>
+  </si>
+  <si>
+    <t>LA Fitness | Gym and Fitness Club | Join Today</t>
   </si>
 </sst>
 </file>
@@ -446,7 +467,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -461,7 +482,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -742,11 +762,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CS7"/>
+  <dimension ref="A1:CS10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
+      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1230,7 +1250,7 @@
         <v>103</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D5" t="s">
         <v>101</v>
@@ -1238,7 +1258,7 @@
       <c r="F5" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="BX5" s="6" t="s">
+      <c r="BX5" t="s">
         <v>113</v>
       </c>
     </row>
@@ -1250,7 +1270,7 @@
         <v>103</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D6" t="s">
         <v>109</v>
@@ -1272,14 +1292,59 @@
       <c r="B7" t="s">
         <v>103</v>
       </c>
-      <c r="C7" t="s">
-        <v>78</v>
+      <c r="C7" s="1" t="s">
+        <v>77</v>
       </c>
       <c r="D7" t="s">
         <v>110</v>
       </c>
       <c r="F7" t="s">
         <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>117</v>
+      </c>
+      <c r="B8" t="s">
+        <v>103</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F8" t="s">
+        <v>120</v>
+      </c>
+      <c r="BX8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>118</v>
+      </c>
+      <c r="B9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F9" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>119</v>
+      </c>
+      <c r="B10" t="s">
+        <v>103</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F10" t="s">
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>